<commit_message>
Add ticket scraping functions for various artists and reduce retry attempts to 5
</commit_message>
<xml_diff>
--- a/Tick_Num.xlsx
+++ b/Tick_Num.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fastb\Desktop\Programming\PROJECTS\Scalping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyData\Programming\PROJECTS\Scalping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B380A8CA-3720-47AF-9D18-84DD05D92DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F93CD2D-0875-4C14-BA3A-F840F3FE3918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="15660" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3190" yWindow="4200" windowWidth="19200" windowHeight="10850" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taylor" sheetId="1" r:id="rId1"/>
     <sheet name="Coldplay" sheetId="2" r:id="rId2"/>
     <sheet name="Adele" sheetId="3" r:id="rId3"/>
     <sheet name="Dua" sheetId="4" r:id="rId4"/>
+    <sheet name="Eilish" sheetId="5" r:id="rId5"/>
+    <sheet name="Carpenter" sheetId="6" r:id="rId6"/>
+    <sheet name="Rodrigo" sheetId="7" r:id="rId7"/>
+    <sheet name="Beyonce" sheetId="8" r:id="rId8"/>
+    <sheet name="Cabello" sheetId="10" r:id="rId9"/>
+    <sheet name="Metallica" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -341,11 +347,31 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA445766-3BD5-4B8F-8C39-2F6BA8726179}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -359,9 +385,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>44</v>
       </c>
@@ -379,9 +405,9 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>10</v>
       </c>
@@ -395,11 +421,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>55</v>
       </c>
@@ -407,4 +433,98 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C39E0D-BA5F-4F58-87BF-03363861C4D4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA594501-CE2B-48E0-82CE-5351031B89E3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>